<commit_message>
Seconde commit SQL Query
</commit_message>
<xml_diff>
--- a/MyAgendas-API-Docs.xlsx
+++ b/MyAgendas-API-Docs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin\Desktop\.IUT-Cours\2A\Web\MyAgendas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EF1EF8-826D-480E-8367-2BF5604B5E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA906048-2E39-435A-9352-02BB58C1BCBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,7 +345,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -355,6 +355,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -488,7 +494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -535,6 +541,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -819,9 +834,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -862,7 +877,7 @@
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -884,7 +899,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -902,7 +917,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -920,7 +935,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -940,6 +955,7 @@
       <c r="I5" s="10" t="s">
         <v>44</v>
       </c>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
@@ -966,7 +982,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -984,10 +1000,11 @@
       <c r="I7" s="10" t="s">
         <v>47</v>
       </c>
+      <c r="J7" s="21"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="23" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -1008,7 +1025,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1029,7 +1046,7 @@
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="11"/>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="24" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="13" t="s">
@@ -1050,7 +1067,7 @@
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="22" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1071,7 +1088,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1088,7 +1105,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="9" t="s">

</xml_diff>